<commit_message>
QA Fixes; Added KRA to Int'l Resources; GRCW-959; RTTBC25 Week 14 Results
</commit_message>
<xml_diff>
--- a/pdf/RTTBC25-Schedule-by-Division_2025-08-16.xlsx
+++ b/pdf/RTTBC25-Schedule-by-Division_2025-08-16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1286" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD27C662-E0EE-424E-9446-E8D13A4752E4}"/>
+  <xr:revisionPtr revIDLastSave="1289" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18BB524B-4D22-4B24-872C-C7B6CC9FEA0D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
+    <workbookView xWindow="21405" yWindow="60" windowWidth="16905" windowHeight="20565" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -257,9 +257,6 @@
     <t>Zenyatta S.-G2</t>
   </si>
   <si>
-    <t>Darley Alcibiades S.-G1</t>
-  </si>
-  <si>
     <t>S. K. Ogden Phoenix S.-G2</t>
   </si>
   <si>
@@ -272,15 +269,9 @@
     <t>American Pharoah S.-G1</t>
   </si>
   <si>
-    <t>Claiborne Breed. Fut.-G1</t>
-  </si>
-  <si>
     <t>Beldame S.-G2</t>
   </si>
   <si>
-    <t>Juddmonte Spinster S.-G1</t>
-  </si>
-  <si>
     <t>T'bred Club of America S.-G2</t>
   </si>
   <si>
@@ -372,6 +363,15 @@
   </si>
   <si>
     <t>Goodwood S.-G1</t>
+  </si>
+  <si>
+    <t>Spinster S.-G1</t>
+  </si>
+  <si>
+    <t>Breeders Futurity-G1</t>
+  </si>
+  <si>
+    <t>Alcibiades S.-G1</t>
   </si>
 </sst>
 </file>
@@ -832,15 +832,105 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -856,9 +946,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -868,101 +955,14 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1289,65 +1289,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1783450-6415-4D0D-A0B8-DEE615502A89}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32:E35"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-    </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="75" t="s">
-        <v>94</v>
+    <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="89"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="98" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="100" t="s">
+        <v>91</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E2" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="75"/>
+    </row>
+    <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="100"/>
       <c r="B3" s="32"/>
       <c r="C3" s="30" t="s">
         <v>5</v>
@@ -1371,9 +1371,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="75"/>
-      <c r="B4" s="69">
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="100"/>
+      <c r="B4" s="72">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1382,50 +1382,50 @@
       <c r="D4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="81" t="s">
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="76" t="s">
-        <v>95</v>
+      <c r="H4" s="57" t="s">
+        <v>92</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="75"/>
-      <c r="B5" s="70"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="100"/>
+      <c r="B5" s="73"/>
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="77"/>
+        <v>107</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="58"/>
       <c r="I5" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="75"/>
-      <c r="B6" s="70"/>
+    <row r="6" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="100"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="12"/>
       <c r="D6" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="77"/>
+        <v>103</v>
+      </c>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="21"/>
     </row>
-    <row r="7" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="75"/>
+    <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="100"/>
       <c r="B7" s="33">
         <v>2</v>
       </c>
@@ -1441,8 +1441,8 @@
       <c r="H7" s="15"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="75"/>
+    <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="100"/>
       <c r="B8" s="33">
         <v>3</v>
       </c>
@@ -1454,12 +1454,12 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="51" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" s="48" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="75"/>
+    <row r="9" spans="1:9" s="48" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="100"/>
       <c r="B9" s="38">
         <v>4</v>
       </c>
@@ -1474,60 +1474,60 @@
       <c r="G9" s="36"/>
       <c r="H9" s="45"/>
       <c r="I9" s="36" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="75"/>
-      <c r="B10" s="69">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="100"/>
+      <c r="B10" s="72">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="85" t="s">
+      <c r="E10" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="83"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="68"/>
       <c r="H10" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="83"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="75"/>
-      <c r="B11" s="70"/>
+      <c r="I10" s="68"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="100"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="84"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="84"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="84"/>
-    </row>
-    <row r="12" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="75"/>
-      <c r="B12" s="70"/>
+      <c r="I11" s="69"/>
+    </row>
+    <row r="12" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="100"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="84"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="84"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="37"/>
-      <c r="I12" s="84"/>
-    </row>
-    <row r="13" spans="1:9" ht="18.600000000000001" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="75"/>
+      <c r="I12" s="69"/>
+    </row>
+    <row r="13" spans="1:9" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="100"/>
       <c r="B13" s="33">
         <v>6</v>
       </c>
@@ -1539,9 +1539,9 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="75"/>
-      <c r="B14" s="69">
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="100"/>
+      <c r="B14" s="72">
         <v>7</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1550,116 +1550,116 @@
       <c r="D14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="76" t="s">
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="76" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="75"/>
-      <c r="B15" s="70"/>
+      <c r="I14" s="57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="100"/>
+      <c r="B15" s="73"/>
       <c r="C15" s="19" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-    </row>
-    <row r="16" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="75"/>
-      <c r="B16" s="80"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+    </row>
+    <row r="16" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="100"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="12"/>
       <c r="D16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="75"/>
-      <c r="B17" s="69">
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="100"/>
+      <c r="B17" s="72">
         <v>8</v>
       </c>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="99" t="s">
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="58"/>
+      <c r="H17" s="62"/>
       <c r="I17" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="75"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="72"/>
+    <row r="18" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="100"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="64"/>
       <c r="I18" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A19" s="75"/>
-      <c r="B19" s="69">
+    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A19" s="100"/>
+      <c r="B19" s="72">
         <v>9</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="81" t="s">
+      <c r="D19" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="76" t="s">
+      <c r="E19" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="83" t="s">
+      <c r="F19" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="58"/>
-      <c r="H19" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19" s="58"/>
-    </row>
-    <row r="20" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="75"/>
-      <c r="B20" s="70"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="I19" s="62"/>
+    </row>
+    <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="100"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="82"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="84"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="59"/>
-    </row>
-    <row r="21" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="75"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="63"/>
+    </row>
+    <row r="21" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="100"/>
       <c r="B21" s="38">
         <v>10</v>
       </c>
@@ -1675,8 +1675,8 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="75"/>
+    <row r="22" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="100"/>
       <c r="B22" s="38">
         <v>11</v>
       </c>
@@ -1692,97 +1692,97 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A23" s="75"/>
-      <c r="B23" s="69">
+    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A23" s="100"/>
+      <c r="B23" s="72">
         <v>12</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="81" t="s">
+      <c r="D23" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="58"/>
-      <c r="F23" s="85"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="65"/>
       <c r="G23" s="20" t="s">
         <v>45</v>
       </c>
       <c r="H23" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="I23" s="58"/>
-    </row>
-    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A24" s="75"/>
-      <c r="B24" s="70"/>
+      <c r="I23" s="62"/>
+    </row>
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="100"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="82"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="86"/>
+        <v>94</v>
+      </c>
+      <c r="D24" s="60"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="66"/>
       <c r="G24" s="21" t="s">
         <v>46</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="59"/>
-    </row>
-    <row r="25" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="75"/>
-      <c r="B25" s="80"/>
+      <c r="I24" s="63"/>
+    </row>
+    <row r="25" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="100"/>
+      <c r="B25" s="74"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="100"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="67"/>
       <c r="G25" s="14" t="s">
         <v>49</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="I25" s="72"/>
-    </row>
-    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="75"/>
-      <c r="B26" s="69">
+        <v>99</v>
+      </c>
+      <c r="I25" s="64"/>
+    </row>
+    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A26" s="100"/>
+      <c r="B26" s="72">
         <v>13</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="83" t="s">
+      <c r="D26" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="78" t="s">
+      <c r="E26" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="81" t="s">
+      <c r="F26" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="58"/>
-      <c r="H26" s="83" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" s="58"/>
-    </row>
-    <row r="27" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="75"/>
-      <c r="B27" s="80"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="I26" s="62"/>
+    </row>
+    <row r="27" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="100"/>
+      <c r="B27" s="74"/>
       <c r="C27" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="72"/>
-    </row>
-    <row r="28" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="75"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="64"/>
+    </row>
+    <row r="28" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="100"/>
       <c r="B28" s="33">
         <v>14</v>
       </c>
@@ -1798,14 +1798,14 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="75"/>
+    <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="100"/>
       <c r="B29" s="33">
         <v>15</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E29" s="27" t="s">
         <v>57</v>
@@ -1817,45 +1817,45 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A30" s="75"/>
-      <c r="B30" s="69">
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="100"/>
+      <c r="B30" s="72">
         <v>16</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="78" t="s">
+      <c r="D30" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="85"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="62"/>
       <c r="H30" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="I30" s="76" t="s">
+      <c r="I30" s="57" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="75"/>
-      <c r="B31" s="70"/>
+    <row r="31" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="100"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="79"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
+      <c r="D31" s="88"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
       <c r="H31" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="I31" s="77"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="75"/>
-      <c r="B32" s="69">
+        <v>93</v>
+      </c>
+      <c r="I31" s="58"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="100"/>
+      <c r="B32" s="72">
         <v>17</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -1864,120 +1864,120 @@
       <c r="D32" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="67" t="s">
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="H32" s="76" t="s">
+      <c r="H32" s="57" t="s">
         <v>67</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A33" s="75"/>
-      <c r="B33" s="70"/>
+    <row r="33" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A33" s="100"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="77"/>
+        <v>104</v>
+      </c>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="58"/>
       <c r="I33" s="55" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="75"/>
-      <c r="B34" s="70"/>
+    <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="100"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="94"/>
-    </row>
-    <row r="35" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="75"/>
-      <c r="B35" s="70"/>
+      <c r="D34" s="99" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="79"/>
+    </row>
+    <row r="35" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="100"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="74"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="95"/>
-    </row>
-    <row r="36" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="75"/>
-      <c r="B36" s="69">
+      <c r="D35" s="85"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="80"/>
+    </row>
+    <row r="36" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="100"/>
+      <c r="B36" s="72">
         <v>18</v>
       </c>
-      <c r="C36" s="91"/>
+      <c r="C36" s="75"/>
       <c r="D36" s="53"/>
       <c r="E36" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="62"/>
+      <c r="H36" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="I36" s="81" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A37" s="100"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G36" s="58"/>
-      <c r="H36" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="I36" s="96" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A37" s="75"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="G37" s="59"/>
+      <c r="G37" s="63"/>
       <c r="H37" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="I37" s="97"/>
-    </row>
-    <row r="38" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="75"/>
-      <c r="B38" s="80"/>
-      <c r="C38" s="93"/>
+      <c r="I37" s="82"/>
+    </row>
+    <row r="38" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="100"/>
+      <c r="B38" s="74"/>
+      <c r="C38" s="77"/>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G38" s="72"/>
+        <v>100</v>
+      </c>
+      <c r="G38" s="64"/>
       <c r="H38" s="43"/>
-      <c r="I38" s="98"/>
-    </row>
-    <row r="39" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="75"/>
+      <c r="I38" s="83"/>
+    </row>
+    <row r="39" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="100"/>
       <c r="B39" s="33">
         <v>20</v>
       </c>
@@ -1987,27 +1987,27 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A40" s="57"/>
-      <c r="B40" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="65"/>
-      <c r="I40" s="66"/>
-    </row>
-    <row r="41" spans="1:9" s="16" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="57"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A40" s="89"/>
+      <c r="B40" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="71"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="95"/>
+    </row>
+    <row r="41" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="89"/>
       <c r="B41" s="18"/>
       <c r="C41" s="17">
         <f>COUNTIF(C4:C39, "&lt;&gt;")</f>
@@ -2038,48 +2038,78 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="57"/>
-      <c r="B42" s="65" t="str">
+    <row r="42" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="89"/>
+      <c r="B42" s="71" t="str">
         <f>SUM(C41:I41) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
         <v>94 Total Races (Prior to Breeders' Cup Weekend)</v>
       </c>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-    </row>
-    <row r="43" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="57"/>
-      <c r="B43" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="62" t="s">
-        <v>91</v>
-      </c>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
-      <c r="I43" s="64"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+    </row>
+    <row r="43" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="89"/>
+      <c r="B43" s="90" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="90"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="91"/>
+      <c r="F43" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" s="93"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="G32:G35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A2:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E23:E25"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="G10:G12"/>
@@ -2096,47 +2126,17 @@
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="H32:H35"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="G32:G35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A2:A39"/>
-    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G26:G27"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" fitToHeight="10" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>